<commit_message>
Updated and removed unnecessary code
</commit_message>
<xml_diff>
--- a/Wolf-Fuels.xlsx
+++ b/Wolf-Fuels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uncommonStudent\Desktop\PYTHON_PROJECTS\Payslip Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531E1D15-8A65-4A58-8C3A-81FC5192DAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E54D8B0-9257-4465-8652-D8A2132B2CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{17C70322-96B8-4C06-A2FA-C71F050071F7}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t xml:space="preserve">Reece Kurangwa </t>
   </si>
   <si>
-    <t>nicolaskudzai696@gmail.com</t>
-  </si>
-  <si>
     <t>lloyddonnel44@gmail.com</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t xml:space="preserve">Names </t>
+  </si>
+  <si>
+    <t>kudziet221@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -178,11 +178,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,7 +502,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="112" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,16 +517,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -538,11 +539,11 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>1200</v>
@@ -559,10 +560,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>1500</v>
@@ -576,13 +577,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>1100</v>

</xml_diff>